<commit_message>
Remove external linking and update the fill table
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED-Halfway.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED-Halfway.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIM-2.0\TIMES-Ireland-model-CB\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F508959-8C0C-41AC-AA0D-628CCA339693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2BCC61-CB24-47CC-9A29-A77B9DA1E46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY-Demands" sheetId="5" r:id="rId1"/>
@@ -20,9 +20,6 @@
     <sheet name="Residential" sheetId="8" r:id="rId5"/>
     <sheet name="Services" sheetId="9" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="1" hidden="1">#REF!</definedName>
@@ -971,7 +968,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1015,11 +1012,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -1057,7 +1051,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>31750</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1105,29 +1099,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="BY-Demands"/>
-      <sheetName val="REG_TRA_DEMANDS"/>
-      <sheetName val="Regions"/>
-      <sheetName val="DEMANDS"/>
-      <sheetName val="Residential"/>
-      <sheetName val="Services"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1395,25 +1366,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0226CF39-0357-4B21-823B-1B3093B14EE8}">
   <dimension ref="C4:AK42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="9.1796875" style="3"/>
-    <col min="7" max="7" width="10.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="3"/>
-    <col min="9" max="9" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="6" width="9.140625" style="3"/>
+    <col min="7" max="7" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="3"/>
+    <col min="9" max="9" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:37" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="4" t="s">
         <v>63</v>
       </c>
@@ -1548,7 +1519,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>66</v>
       </c>
@@ -1647,7 +1618,7 @@
         <v>0.20769618859639599</v>
       </c>
     </row>
-    <row r="7" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>66</v>
       </c>
@@ -1746,7 +1717,7 @@
         <v>0.47664625412085698</v>
       </c>
     </row>
-    <row r="8" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>66</v>
       </c>
@@ -1845,7 +1816,7 @@
         <v>0.42809298937083901</v>
       </c>
     </row>
-    <row r="9" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>66</v>
       </c>
@@ -1944,7 +1915,7 @@
         <v>0.154582741264056</v>
       </c>
     </row>
-    <row r="10" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>66</v>
       </c>
@@ -2043,7 +2014,7 @@
         <v>9.95787628254481E-2</v>
       </c>
     </row>
-    <row r="11" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>66</v>
       </c>
@@ -2142,7 +2113,7 @@
         <v>4.5290536808279797E-2</v>
       </c>
     </row>
-    <row r="12" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>66</v>
       </c>
@@ -2241,7 +2212,7 @@
         <v>0.28082969344526898</v>
       </c>
     </row>
-    <row r="13" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>66</v>
       </c>
@@ -2340,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>66</v>
       </c>
@@ -2439,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>66</v>
       </c>
@@ -2488,7 +2459,7 @@
       <c r="AJ15" s="22"/>
       <c r="AK15" s="22"/>
     </row>
-    <row r="16" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>66</v>
       </c>
@@ -2537,7 +2508,7 @@
       <c r="AJ16" s="22"/>
       <c r="AK16" s="22"/>
     </row>
-    <row r="17" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>66</v>
       </c>
@@ -2586,7 +2557,7 @@
       <c r="AJ17" s="22"/>
       <c r="AK17" s="22"/>
     </row>
-    <row r="18" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>66</v>
       </c>
@@ -2635,7 +2606,7 @@
       <c r="AJ18" s="22"/>
       <c r="AK18" s="22"/>
     </row>
-    <row r="19" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>66</v>
       </c>
@@ -2684,7 +2655,7 @@
       <c r="AJ19" s="22"/>
       <c r="AK19" s="22"/>
     </row>
-    <row r="20" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
         <v>66</v>
       </c>
@@ -2733,7 +2704,7 @@
       <c r="AJ20" s="22"/>
       <c r="AK20" s="22"/>
     </row>
-    <row r="21" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>66</v>
       </c>
@@ -2782,7 +2753,7 @@
       <c r="AJ21" s="22"/>
       <c r="AK21" s="22"/>
     </row>
-    <row r="22" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>66</v>
       </c>
@@ -2831,7 +2802,7 @@
       <c r="AJ22" s="22"/>
       <c r="AK22" s="22"/>
     </row>
-    <row r="23" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>66</v>
       </c>
@@ -2880,7 +2851,7 @@
       <c r="AJ23" s="22"/>
       <c r="AK23" s="22"/>
     </row>
-    <row r="24" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>66</v>
       </c>
@@ -2929,7 +2900,7 @@
       <c r="AJ24" s="22"/>
       <c r="AK24" s="22"/>
     </row>
-    <row r="25" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>66</v>
       </c>
@@ -2978,7 +2949,7 @@
       <c r="AJ25" s="22"/>
       <c r="AK25" s="22"/>
     </row>
-    <row r="26" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>66</v>
       </c>
@@ -3027,7 +2998,7 @@
       <c r="AJ26" s="22"/>
       <c r="AK26" s="22"/>
     </row>
-    <row r="27" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
         <v>66</v>
       </c>
@@ -3076,7 +3047,7 @@
       <c r="AJ27" s="22"/>
       <c r="AK27" s="22"/>
     </row>
-    <row r="28" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="s">
         <v>66</v>
       </c>
@@ -3125,7 +3096,7 @@
       <c r="AJ28" s="22"/>
       <c r="AK28" s="22"/>
     </row>
-    <row r="29" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>66</v>
       </c>
@@ -3174,7 +3145,7 @@
       <c r="AJ29" s="22"/>
       <c r="AK29" s="22"/>
     </row>
-    <row r="30" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
         <v>66</v>
       </c>
@@ -3223,7 +3194,7 @@
       <c r="AJ30" s="22"/>
       <c r="AK30" s="22"/>
     </row>
-    <row r="31" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
         <v>66</v>
       </c>
@@ -3272,7 +3243,7 @@
       <c r="AJ31" s="22"/>
       <c r="AK31" s="22"/>
     </row>
-    <row r="32" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
         <v>66</v>
       </c>
@@ -3321,7 +3292,7 @@
       <c r="AJ32" s="22"/>
       <c r="AK32" s="22"/>
     </row>
-    <row r="33" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
@@ -3370,7 +3341,7 @@
       <c r="AJ33" s="22"/>
       <c r="AK33" s="22"/>
     </row>
-    <row r="34" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C34" s="3" t="s">
         <v>66</v>
       </c>
@@ -3419,7 +3390,7 @@
       <c r="AJ34" s="22"/>
       <c r="AK34" s="22"/>
     </row>
-    <row r="35" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
         <v>66</v>
       </c>
@@ -3468,7 +3439,7 @@
       <c r="AJ35" s="22"/>
       <c r="AK35" s="22"/>
     </row>
-    <row r="36" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C36" s="3" t="s">
         <v>66</v>
       </c>
@@ -3517,7 +3488,7 @@
       <c r="AJ36" s="22"/>
       <c r="AK36" s="22"/>
     </row>
-    <row r="37" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C37" s="3" t="s">
         <v>66</v>
       </c>
@@ -3566,7 +3537,7 @@
       <c r="AJ37" s="22"/>
       <c r="AK37" s="22"/>
     </row>
-    <row r="38" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C38" s="3" t="s">
         <v>66</v>
       </c>
@@ -3615,7 +3586,7 @@
       <c r="AJ38" s="22"/>
       <c r="AK38" s="22"/>
     </row>
-    <row r="39" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C39" s="3" t="s">
         <v>66</v>
       </c>
@@ -3660,7 +3631,7 @@
       <c r="AJ39" s="22"/>
       <c r="AK39" s="22"/>
     </row>
-    <row r="40" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C40" s="3" t="s">
         <v>66</v>
       </c>
@@ -3705,7 +3676,7 @@
       <c r="AJ40" s="22"/>
       <c r="AK40" s="22"/>
     </row>
-    <row r="41" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C41" s="3" t="s">
         <v>66</v>
       </c>
@@ -3754,7 +3725,7 @@
       <c r="AJ41" s="22"/>
       <c r="AK41" s="22"/>
     </row>
-    <row r="42" spans="3:37" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:37" ht="15" x14ac:dyDescent="0.25">
       <c r="C42" s="3" t="s">
         <v>66</v>
       </c>
@@ -3814,22 +3785,22 @@
   <dimension ref="B2:AF39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9.1796875" style="3"/>
-    <col min="4" max="4" width="11.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="2:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>65</v>
       </c>
@@ -3950,7 +3921,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="2:32" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D4" s="3" t="s">
         <v>59</v>
       </c>
@@ -4066,7 +4037,7 @@
         <v>0.2122596962048626</v>
       </c>
     </row>
-    <row r="5" spans="2:32" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D5" s="3" t="s">
         <v>59</v>
       </c>
@@ -4182,7 +4153,7 @@
         <v>0.15354445783325901</v>
       </c>
     </row>
-    <row r="6" spans="2:32" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
         <v>59</v>
       </c>
@@ -4298,7 +4269,7 @@
         <v>0.19657172711717047</v>
       </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D7" s="3" t="s">
         <v>59</v>
       </c>
@@ -4414,7 +4385,7 @@
         <v>0.28262626568499355</v>
       </c>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D8" s="3" t="s">
         <v>59</v>
       </c>
@@ -4530,7 +4501,7 @@
         <v>0.48743823497682215</v>
       </c>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D9" s="3" t="s">
         <v>59</v>
       </c>
@@ -4646,7 +4617,7 @@
         <v>0.35260315962707711</v>
       </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D10" s="3" t="s">
         <v>59</v>
       </c>
@@ -4762,7 +4733,7 @@
         <v>0.42633640999216782</v>
       </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D11" s="3" t="s">
         <v>59</v>
       </c>
@@ -4878,7 +4849,7 @@
         <v>0.57380291072234901</v>
       </c>
     </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D12" s="3" t="s">
         <v>59</v>
       </c>
@@ -4994,7 +4965,7 @@
         <v>0.43424277040967463</v>
       </c>
     </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D13" s="3" t="s">
         <v>59</v>
       </c>
@@ -5110,7 +5081,7 @@
         <v>0.31412261464919838</v>
       </c>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D14" s="3" t="s">
         <v>59</v>
       </c>
@@ -5226,7 +5197,7 @@
         <v>0.37971547763938718</v>
       </c>
     </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D15" s="3" t="s">
         <v>59</v>
       </c>
@@ -5342,7 +5313,7 @@
         <v>0.51090120361976454</v>
       </c>
     </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:32" x14ac:dyDescent="0.2">
       <c r="D16" s="3" t="s">
         <v>59</v>
       </c>
@@ -5458,7 +5429,7 @@
         <v>0.18922217409036649</v>
       </c>
     </row>
-    <row r="17" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D17" s="3" t="s">
         <v>59</v>
       </c>
@@ -5574,7 +5545,7 @@
         <v>0.15629751581539669</v>
       </c>
     </row>
-    <row r="18" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D18" s="3" t="s">
         <v>59</v>
       </c>
@@ -5690,7 +5661,7 @@
         <v>0.18085039009610454</v>
       </c>
     </row>
-    <row r="19" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D19" s="3" t="s">
         <v>59</v>
       </c>
@@ -5806,7 +5777,7 @@
         <v>0.22995613865752026</v>
       </c>
     </row>
-    <row r="20" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D20" s="3" t="s">
         <v>59</v>
       </c>
@@ -5922,7 +5893,7 @@
         <v>0.14086885317580392</v>
       </c>
     </row>
-    <row r="21" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D21" s="3" t="s">
         <v>59</v>
       </c>
@@ -6037,7 +6008,7 @@
         <v>0.12806259379618537</v>
       </c>
     </row>
-    <row r="22" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D22" s="3" t="s">
         <v>59</v>
       </c>
@@ -6152,7 +6123,7 @@
         <v>8.5375062530790247E-2</v>
       </c>
     </row>
-    <row r="23" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D23" s="3" t="s">
         <v>59</v>
       </c>
@@ -6267,7 +6238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D24" s="3" t="s">
         <v>59</v>
       </c>
@@ -6383,7 +6354,7 @@
         <v>5.5388643974572375E-2</v>
       </c>
     </row>
-    <row r="25" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D25" s="3" t="s">
         <v>59</v>
       </c>
@@ -6498,7 +6469,7 @@
         <v>5.6842758875006623E-2</v>
       </c>
     </row>
-    <row r="26" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D26" s="3" t="s">
         <v>59</v>
       </c>
@@ -6613,7 +6584,7 @@
         <v>6.7013553434566345E-2</v>
       </c>
     </row>
-    <row r="27" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D27" s="3" t="s">
         <v>59</v>
       </c>
@@ -6728,7 +6699,7 @@
         <v>8.7355142553685775E-2</v>
       </c>
     </row>
-    <row r="28" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D28" s="3" t="s">
         <v>59</v>
       </c>
@@ -6844,7 +6815,7 @@
         <v>0.17571155329873456</v>
       </c>
     </row>
-    <row r="29" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D29" s="3" t="s">
         <v>59</v>
       </c>
@@ -6960,7 +6931,7 @@
         <v>0.17505912318297531</v>
       </c>
     </row>
-    <row r="30" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D30" s="3" t="s">
         <v>59</v>
       </c>
@@ -7076,7 +7047,7 @@
         <v>0.11670608212198352</v>
       </c>
     </row>
-    <row r="31" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D31" s="3" t="s">
         <v>59</v>
       </c>
@@ -7192,7 +7163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D32" s="3" t="s">
         <v>59</v>
       </c>
@@ -7308,7 +7279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D33" s="3" t="s">
         <v>59</v>
       </c>
@@ -7423,7 +7394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D34" s="3" t="s">
         <v>59</v>
       </c>
@@ -7538,7 +7509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D35" s="3" t="s">
         <v>59</v>
       </c>
@@ -7653,7 +7624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D36" s="3" t="s">
         <v>59</v>
       </c>
@@ -7769,7 +7740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D37" s="3" t="s">
         <v>59</v>
       </c>
@@ -7885,7 +7856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D38" s="3" t="s">
         <v>59</v>
       </c>
@@ -8001,7 +7972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:32" x14ac:dyDescent="0.2">
       <c r="D39" s="3" t="s">
         <v>59</v>
       </c>
@@ -8130,38 +8101,38 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="3.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.54296875" style="3" customWidth="1"/>
-    <col min="25" max="25" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.1796875" style="3"/>
+    <col min="29" max="29" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="C3" s="19" t="str">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -8275,12 +8246,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>133</v>
       </c>
@@ -8395,7 +8366,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>132</v>
       </c>
@@ -8512,7 +8483,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>131</v>
       </c>
@@ -8629,7 +8600,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>130</v>
       </c>
@@ -8637,7 +8608,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>76</v>
       </c>
@@ -8645,7 +8616,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>99</v>
       </c>
@@ -8653,7 +8624,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>88</v>
       </c>
@@ -8661,7 +8632,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>89</v>
       </c>
@@ -8669,7 +8640,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>100</v>
       </c>
@@ -8677,7 +8648,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>77</v>
       </c>
@@ -8685,7 +8656,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>94</v>
       </c>
@@ -8693,7 +8664,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>90</v>
       </c>
@@ -8701,7 +8672,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>78</v>
       </c>
@@ -8709,7 +8680,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>79</v>
       </c>
@@ -8717,7 +8688,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>80</v>
       </c>
@@ -8725,7 +8696,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>95</v>
       </c>
@@ -8733,7 +8704,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>91</v>
       </c>
@@ -8741,7 +8712,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>81</v>
       </c>
@@ -8749,7 +8720,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>82</v>
       </c>
@@ -8757,7 +8728,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>96</v>
       </c>
@@ -8765,7 +8736,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>83</v>
       </c>
@@ -8773,7 +8744,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>101</v>
       </c>
@@ -8781,7 +8752,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>84</v>
       </c>
@@ -8789,7 +8760,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>97</v>
       </c>
@@ -8797,7 +8768,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>98</v>
       </c>
@@ -8805,7 +8776,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>92</v>
       </c>
@@ -8813,7 +8784,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>93</v>
       </c>
@@ -8821,7 +8792,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>85</v>
       </c>
@@ -8829,7 +8800,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
         <v>86</v>
       </c>
@@ -8837,7 +8808,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
         <v>87</v>
       </c>
@@ -8845,7 +8816,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>102</v>
       </c>
@@ -8871,7 +8842,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>31750</xdr:colOff>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -8890,27 +8861,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:AQ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.453125" customWidth="1"/>
-    <col min="10" max="11" width="15.81640625" customWidth="1"/>
-    <col min="12" max="12" width="11.7265625" customWidth="1"/>
-    <col min="13" max="13" width="12.81640625" customWidth="1"/>
-    <col min="16" max="16" width="8.81640625" customWidth="1"/>
-    <col min="17" max="17" width="10.54296875" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+    <col min="10" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>149</v>
       </c>
@@ -8918,7 +8889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="3:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
@@ -8986,7 +8957,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D3" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9042,17 +9013,17 @@
       <c r="U3">
         <v>9.7989935307649739E-2</v>
       </c>
-      <c r="V3" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="35">
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="32">
         <v>0.126438626203419</v>
       </c>
       <c r="Z3" s="30">
         <v>6.9541244411880462E-2</v>
       </c>
     </row>
-    <row r="4" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D4" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9108,17 +9079,17 @@
       <c r="U4">
         <v>26.346234207155959</v>
       </c>
-      <c r="V4" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="35">
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="32">
         <v>33.995140912459298</v>
       </c>
       <c r="Z4" s="30">
         <v>18.697327501852616</v>
       </c>
     </row>
-    <row r="5" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D5" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9174,17 +9145,17 @@
       <c r="U5">
         <v>3.8534877653787154</v>
       </c>
-      <c r="V5" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="35">
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="32">
         <v>4.9722422779080198</v>
       </c>
       <c r="Z5" s="30">
         <v>2.7347332528494115</v>
       </c>
     </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9240,17 +9211,17 @@
       <c r="U6">
         <v>5.9308505795404391</v>
       </c>
-      <c r="V6" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="35">
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="32">
         <v>7.6527104252134697</v>
       </c>
       <c r="Z6" s="30">
         <v>4.2089907338674086</v>
       </c>
     </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D7" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9306,17 +9277,17 @@
       <c r="U7">
         <v>1.7912647554770649</v>
       </c>
-      <c r="V7" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="35">
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="32">
         <v>2.3113093619058902</v>
       </c>
       <c r="Z7" s="30">
         <v>1.2712201490482398</v>
       </c>
     </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D8" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9372,17 +9343,17 @@
       <c r="U8">
         <v>10.157935062437405</v>
       </c>
-      <c r="V8" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="35">
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="32">
         <v>13.107012983790201</v>
       </c>
       <c r="Z8" s="30">
         <v>7.2088571410846098</v>
       </c>
     </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D9" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9438,17 +9409,17 @@
       <c r="U9">
         <v>0.68793979220818868</v>
       </c>
-      <c r="V9" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="35">
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="32">
         <v>0.88766424801056598</v>
       </c>
       <c r="Z9" s="30">
         <v>0.48821533640581133</v>
       </c>
     </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D10" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9504,17 +9475,17 @@
       <c r="U10">
         <v>16.853923637480463</v>
       </c>
-      <c r="V10" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="35">
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="32">
         <v>24.822798092583323</v>
       </c>
       <c r="Z10" s="30">
         <v>8.8850491823775997</v>
       </c>
     </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D11" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9570,17 +9541,17 @@
       <c r="U11">
         <v>16.844014653390236</v>
       </c>
-      <c r="V11" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="35">
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="32">
         <v>21.7342124559874</v>
       </c>
       <c r="Z11" s="30">
         <v>11.953816850793071</v>
       </c>
     </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D12" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9636,17 +9607,17 @@
       <c r="U12">
         <v>1.3071809478517049</v>
       </c>
-      <c r="V12" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="35">
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="32">
         <v>1.6866850940022</v>
       </c>
       <c r="Z12" s="30">
         <v>0.92767680170120992</v>
       </c>
     </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D13" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9702,17 +9673,17 @@
       <c r="U13">
         <v>12.686569622394671</v>
       </c>
-      <c r="V13" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="35">
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="32">
         <v>16.369767254702801</v>
       </c>
       <c r="Z13" s="30">
         <v>9.0033719900865421</v>
       </c>
     </row>
-    <row r="14" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D14" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9768,17 +9739,17 @@
       <c r="U14">
         <v>3.2628733640509965E-2</v>
       </c>
-      <c r="V14" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="35">
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="32">
         <v>4.2101591794206403E-2</v>
       </c>
       <c r="Z14" s="30">
         <v>2.3155875486813523E-2</v>
       </c>
     </row>
-    <row r="15" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D15" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9834,17 +9805,17 @@
       <c r="U15">
         <v>4.7394475614649956</v>
       </c>
-      <c r="V15" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="35">
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="32">
         <v>6.1154162083419301</v>
       </c>
       <c r="Z15" s="30">
         <v>3.3634789145880619</v>
       </c>
     </row>
-    <row r="16" spans="3:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D16" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -9900,17 +9871,17 @@
       <c r="U16">
         <v>4.5713249322390208</v>
       </c>
-      <c r="V16" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="35">
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="32">
         <v>5.8984837835342203</v>
       </c>
       <c r="Z16" s="30">
         <v>3.2441660809438213</v>
       </c>
     </row>
-    <row r="17" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D17" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -9966,17 +9937,17 @@
       <c r="U17">
         <v>19.808098215775729</v>
       </c>
-      <c r="V17" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="35">
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="32">
         <v>21.065548257939199</v>
       </c>
       <c r="Z17" s="30">
         <v>18.550648173612263</v>
       </c>
     </row>
-    <row r="18" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D18" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -10032,17 +10003,17 @@
       <c r="U18">
         <v>37.651251214826601</v>
       </c>
-      <c r="V18" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="35">
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="32">
         <v>45.290928754569201</v>
       </c>
       <c r="Z18" s="30">
         <v>30.011573675084005</v>
       </c>
     </row>
-    <row r="19" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D19" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -10098,17 +10069,17 @@
       <c r="U19">
         <v>32.379777214245621</v>
       </c>
-      <c r="V19" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="35">
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="32">
         <v>38.971264277187501</v>
       </c>
       <c r="Z19" s="30">
         <v>25.788290151303741</v>
       </c>
     </row>
-    <row r="20" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D20" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -10164,17 +10135,17 @@
       <c r="U20">
         <v>17.294083387740336</v>
       </c>
-      <c r="V20" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="35">
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="32">
         <v>25.138166775480673</v>
       </c>
       <c r="Z20" s="30">
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="21" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D21" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -10230,17 +10201,17 @@
       <c r="U21">
         <v>0</v>
       </c>
-      <c r="V21" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="35">
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="32">
         <v>0</v>
       </c>
       <c r="Z21" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D22" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -10296,10 +10267,10 @@
       <c r="U22">
         <v>6.7763561055681549</v>
       </c>
-      <c r="V22" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="35">
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="32">
         <v>10.039412402408599</v>
       </c>
       <c r="Z22" s="30">
@@ -10307,7 +10278,7 @@
         <v>3.5132998087277101</v>
       </c>
     </row>
-    <row r="23" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D23" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -10363,17 +10334,17 @@
       <c r="U23">
         <v>0</v>
       </c>
-      <c r="V23" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="35">
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="32">
         <v>0</v>
       </c>
       <c r="Z23" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D24" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -10429,10 +10400,10 @@
       <c r="U24">
         <v>0.23174660014328952</v>
       </c>
-      <c r="V24" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="35">
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="32">
         <v>0.23</v>
       </c>
       <c r="Z24" s="30">
@@ -10440,7 +10411,7 @@
         <v>0.23349320028657899</v>
       </c>
     </row>
-    <row r="25" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D25" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3)</f>
         <v>IE</v>
@@ -10496,10 +10467,10 @@
       <c r="U25">
         <v>54.282828207215999</v>
       </c>
-      <c r="V25" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="35">
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="32">
         <v>62.629819759999997</v>
       </c>
       <c r="Z25" s="30">
@@ -10507,7 +10478,7 @@
         <v>45.935836654432002</v>
       </c>
     </row>
-    <row r="26" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D26" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -10524,37 +10495,37 @@
       <c r="H26" s="31">
         <v>28.901664567933956</v>
       </c>
-      <c r="I26" s="32">
+      <c r="I26" s="30">
         <v>29.285472960899106</v>
       </c>
-      <c r="J26" s="32">
+      <c r="J26" s="30">
         <v>29.618106901468909</v>
       </c>
-      <c r="K26" s="32">
+      <c r="K26" s="30">
         <v>30.592051000616877</v>
       </c>
-      <c r="L26" s="32">
+      <c r="L26" s="30">
         <v>30.871384926093015</v>
       </c>
-      <c r="M26" s="32">
+      <c r="M26" s="30">
         <v>31.150718851569195</v>
       </c>
-      <c r="N26" s="32">
+      <c r="N26" s="30">
         <v>31.430052777045262</v>
       </c>
-      <c r="O26" s="32">
+      <c r="O26" s="30">
         <v>31.709386702521329</v>
       </c>
-      <c r="P26" s="32">
+      <c r="P26" s="30">
         <v>31.988720627997509</v>
       </c>
-      <c r="Q26" s="32">
+      <c r="Q26" s="30">
         <v>32.268054553473576</v>
       </c>
-      <c r="R26" s="32">
+      <c r="R26" s="30">
         <v>32.547388478949642</v>
       </c>
-      <c r="S26" s="32">
+      <c r="S26" s="30">
         <v>32.826722404425709</v>
       </c>
       <c r="T26" s="30">
@@ -10563,17 +10534,17 @@
       <c r="U26">
         <v>40.081955186767516</v>
       </c>
-      <c r="V26" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="35">
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="32">
         <v>47.391759323456121</v>
       </c>
       <c r="Z26" s="30">
         <v>32.772151050078904</v>
       </c>
     </row>
-    <row r="27" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D27" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -10590,37 +10561,37 @@
       <c r="H27" s="31">
         <v>58.151541961987604</v>
       </c>
-      <c r="I27" s="32">
+      <c r="I27" s="30">
         <v>58.923782945423504</v>
       </c>
-      <c r="J27" s="32">
+      <c r="J27" s="30">
         <v>59.593058464401295</v>
       </c>
-      <c r="K27" s="32">
+      <c r="K27" s="30">
         <v>61.552680928952022</v>
       </c>
-      <c r="L27" s="32">
+      <c r="L27" s="30">
         <v>62.117495669376012</v>
       </c>
-      <c r="M27" s="32">
+      <c r="M27" s="30">
         <v>62.682310409800039</v>
       </c>
-      <c r="N27" s="32">
+      <c r="N27" s="30">
         <v>63.247125150224065</v>
       </c>
-      <c r="O27" s="32">
+      <c r="O27" s="30">
         <v>63.811939890647864</v>
       </c>
-      <c r="P27" s="32">
+      <c r="P27" s="30">
         <v>64.37675463107189</v>
       </c>
-      <c r="Q27" s="32">
+      <c r="Q27" s="30">
         <v>64.941569371495916</v>
       </c>
-      <c r="R27" s="32">
+      <c r="R27" s="30">
         <v>65.506384111919942</v>
       </c>
-      <c r="S27" s="32">
+      <c r="S27" s="30">
         <v>66.071198852343969</v>
       </c>
       <c r="T27" s="30">
@@ -10629,17 +10600,17 @@
       <c r="U27">
         <v>80.721923849501025</v>
       </c>
-      <c r="V27" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="35">
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="32">
         <v>95.354503699002038</v>
       </c>
       <c r="Z27" s="30">
         <v>66.089343999999997</v>
       </c>
     </row>
-    <row r="28" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D28" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -10695,17 +10666,17 @@
       <c r="U28">
         <v>30</v>
       </c>
-      <c r="V28" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="35">
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="32">
         <v>40.299999999999997</v>
       </c>
       <c r="Z28" s="30">
         <v>40.299999999999997</v>
       </c>
     </row>
-    <row r="29" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D29" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
@@ -10761,17 +10732,17 @@
       <c r="U29">
         <v>0.5575</v>
       </c>
-      <c r="V29" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y29" s="35">
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="32">
         <v>0.57499999999999996</v>
       </c>
       <c r="Z29" s="30">
         <v>0.54</v>
       </c>
     </row>
-    <row r="30" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>185</v>
       </c>
@@ -10826,17 +10797,17 @@
       <c r="U30">
         <v>1.662610527</v>
       </c>
-      <c r="V30" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y30" s="35">
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="32">
         <v>1.7132210539999999</v>
       </c>
       <c r="Z30" s="30">
         <v>1.6120000000000001</v>
       </c>
     </row>
-    <row r="31" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>185</v>
       </c>
@@ -10891,17 +10862,17 @@
       <c r="U31">
         <v>2.9449756144999997</v>
       </c>
-      <c r="V31" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="35">
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="32">
         <v>3.0339512289999999</v>
       </c>
       <c r="Z31" s="30">
         <v>2.8559999999999999</v>
       </c>
     </row>
-    <row r="32" spans="4:26" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>185</v>
       </c>
@@ -10956,17 +10927,17 @@
       <c r="U32">
         <v>1.065269408</v>
       </c>
-      <c r="V32" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y32" s="35">
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="32">
         <v>1.1705388160000001</v>
       </c>
       <c r="Z32" s="30">
         <v>0.96</v>
       </c>
     </row>
-    <row r="33" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:43" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>185</v>
       </c>
@@ -11021,17 +10992,17 @@
       <c r="U33">
         <v>1.7438610649999999</v>
       </c>
-      <c r="V33" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y33" s="35">
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="32">
         <v>1.56072213</v>
       </c>
       <c r="Z33" s="30">
         <v>1.927</v>
       </c>
     </row>
-    <row r="34" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:43" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>185</v>
       </c>
@@ -11086,17 +11057,17 @@
       <c r="U34">
         <v>1.4083034209999998</v>
       </c>
-      <c r="V34" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="35">
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="32">
         <v>1.2596068419999999</v>
       </c>
       <c r="Z34" s="30">
         <v>1.5569999999999999</v>
       </c>
     </row>
-    <row r="35" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:43" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>185</v>
       </c>
@@ -11151,17 +11122,17 @@
       <c r="U35">
         <v>12.583426795000001</v>
       </c>
-      <c r="V35" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y35" s="35">
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="32">
         <v>13.98185359</v>
       </c>
       <c r="Z35" s="30">
         <v>11.185</v>
       </c>
     </row>
-    <row r="36" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:43" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>185</v>
       </c>
@@ -11216,23 +11187,23 @@
       <c r="U36">
         <v>0</v>
       </c>
-      <c r="V36" s="33">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="35">
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="32">
         <v>0</v>
       </c>
       <c r="Z36" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:43" x14ac:dyDescent="0.25">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:43" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>149</v>
       </c>
@@ -11244,7 +11215,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="3:43" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="3:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="13" t="s">
         <v>1</v>
       </c>
@@ -11369,7 +11340,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:43" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>59</v>
       </c>
@@ -11481,11 +11452,11 @@
       <c r="AP40">
         <v>657.69915193745828</v>
       </c>
-      <c r="AQ40" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="AQ40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:43" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>59</v>
       </c>
@@ -11516,7 +11487,7 @@
       <c r="O41">
         <v>850.96976936716078</v>
       </c>
-      <c r="P41" s="34">
+      <c r="P41">
         <v>861.58177341465773</v>
       </c>
       <c r="Q41">
@@ -11597,11 +11568,11 @@
       <c r="AP41">
         <v>1088.4635021002869</v>
       </c>
-      <c r="AQ41" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="AQ41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:43" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>59</v>
       </c>
@@ -11632,7 +11603,7 @@
       <c r="O42">
         <v>775.98358172975304</v>
       </c>
-      <c r="P42" s="34">
+      <c r="P42">
         <v>779.02688375026401</v>
       </c>
       <c r="Q42">
@@ -11713,41 +11684,41 @@
       <c r="AP42">
         <v>829.02531795313598</v>
       </c>
-      <c r="AQ42" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="3:43" x14ac:dyDescent="0.35">
+      <c r="AQ42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:43" x14ac:dyDescent="0.25">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:43" x14ac:dyDescent="0.25">
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:43" x14ac:dyDescent="0.25">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:43" x14ac:dyDescent="0.25">
       <c r="H46" s="31"/>
       <c r="I46" s="30"/>
       <c r="J46" s="30"/>
       <c r="K46" s="30"/>
     </row>
-    <row r="47" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:43" x14ac:dyDescent="0.25">
       <c r="H47" s="31"/>
       <c r="I47" s="30"/>
       <c r="J47" s="30"/>
       <c r="K47" s="30"/>
     </row>
-    <row r="48" spans="3:43" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:43" x14ac:dyDescent="0.25">
       <c r="H48" s="31"/>
       <c r="I48" s="30"/>
       <c r="J48" s="30"/>
@@ -11765,18 +11736,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E982DE-1A8D-4D0C-9CD3-51B0DFFDA372}">
   <dimension ref="D4:M216"/>
   <sheetViews>
-    <sheetView topLeftCell="B152" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:K216"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="25" t="s">
         <v>150</v>
       </c>
@@ -11784,7 +11755,7 @@
       <c r="K4" s="26"/>
       <c r="L4" s="26"/>
     </row>
-    <row r="5" spans="4:13" ht="26" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D5" s="27" t="s">
         <v>65</v>
       </c>
@@ -11801,7 +11772,7 @@
         <v>58</v>
       </c>
       <c r="I5" s="27" t="str">
-        <f>IF([1]Regions!AJ5&lt;&gt;"",[1]Regions!AJ5,"*")</f>
+        <f>IF(Regions!AJ5&lt;&gt;"",Regions!AJ5,"*")</f>
         <v>*</v>
       </c>
       <c r="J5" s="27" t="s">
@@ -11817,7 +11788,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D6" s="28" t="s">
         <v>153</v>
       </c>
@@ -11833,7 +11804,7 @@
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
     </row>
-    <row r="7" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>154</v>
       </c>
@@ -11856,7 +11827,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>154</v>
       </c>
@@ -11879,7 +11850,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>154</v>
       </c>
@@ -11902,7 +11873,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>154</v>
       </c>
@@ -11925,7 +11896,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>154</v>
       </c>
@@ -11948,7 +11919,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>154</v>
       </c>
@@ -11971,7 +11942,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>154</v>
       </c>
@@ -11994,7 +11965,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>154</v>
       </c>
@@ -12017,7 +11988,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>154</v>
       </c>
@@ -12040,7 +12011,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="4:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:13" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>154</v>
       </c>
@@ -12063,7 +12034,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>154</v>
       </c>
@@ -12086,7 +12057,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>154</v>
       </c>
@@ -12109,7 +12080,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>154</v>
       </c>
@@ -12132,7 +12103,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>154</v>
       </c>
@@ -12155,7 +12126,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>154</v>
       </c>
@@ -12178,7 +12149,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>154</v>
       </c>
@@ -12201,7 +12172,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>154</v>
       </c>
@@ -12224,7 +12195,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>154</v>
       </c>
@@ -12247,7 +12218,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>154</v>
       </c>
@@ -12270,7 +12241,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>154</v>
       </c>
@@ -12293,7 +12264,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>154</v>
       </c>
@@ -12316,7 +12287,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>159</v>
       </c>
@@ -12342,7 +12313,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>159</v>
       </c>
@@ -12368,7 +12339,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>159</v>
       </c>
@@ -12394,7 +12365,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>159</v>
       </c>
@@ -12420,7 +12391,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>159</v>
       </c>
@@ -12446,7 +12417,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>159</v>
       </c>
@@ -12472,7 +12443,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>159</v>
       </c>
@@ -12498,7 +12469,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>159</v>
       </c>
@@ -12524,7 +12495,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>159</v>
       </c>
@@ -12550,7 +12521,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>159</v>
       </c>
@@ -12576,7 +12547,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>159</v>
       </c>
@@ -12602,7 +12573,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>159</v>
       </c>
@@ -12628,7 +12599,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>159</v>
       </c>
@@ -12654,7 +12625,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>159</v>
       </c>
@@ -12680,7 +12651,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>159</v>
       </c>
@@ -12706,7 +12677,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>159</v>
       </c>
@@ -12732,7 +12703,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>159</v>
       </c>
@@ -12758,7 +12729,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>159</v>
       </c>
@@ -12784,7 +12755,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>159</v>
       </c>
@@ -12810,7 +12781,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>159</v>
       </c>
@@ -12836,7 +12807,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>159</v>
       </c>
@@ -12862,7 +12833,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="49" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
         <v>154</v>
       </c>
@@ -12885,7 +12856,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="50" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
         <v>154</v>
       </c>
@@ -12908,7 +12879,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
         <v>154</v>
       </c>
@@ -12931,7 +12902,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="52" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
         <v>154</v>
       </c>
@@ -12954,7 +12925,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="53" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
         <v>154</v>
       </c>
@@ -12977,7 +12948,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
         <v>154</v>
       </c>
@@ -13000,7 +12971,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="55" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
         <v>154</v>
       </c>
@@ -13023,7 +12994,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="56" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
         <v>154</v>
       </c>
@@ -13046,7 +13017,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
         <v>154</v>
       </c>
@@ -13069,7 +13040,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="58" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
         <v>154</v>
       </c>
@@ -13092,7 +13063,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
         <v>154</v>
       </c>
@@ -13115,7 +13086,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
         <v>154</v>
       </c>
@@ -13138,7 +13109,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="61" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F61" t="s">
         <v>154</v>
       </c>
@@ -13161,7 +13132,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F62" t="s">
         <v>154</v>
       </c>
@@ -13184,7 +13155,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="63" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F63" t="s">
         <v>154</v>
       </c>
@@ -13207,7 +13178,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
         <v>154</v>
       </c>
@@ -13230,7 +13201,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F65" t="s">
         <v>154</v>
       </c>
@@ -13253,7 +13224,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="66" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
         <v>154</v>
       </c>
@@ -13276,7 +13247,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="67" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
         <v>154</v>
       </c>
@@ -13299,7 +13270,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="68" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
         <v>154</v>
       </c>
@@ -13322,7 +13293,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="69" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F69" t="s">
         <v>154</v>
       </c>
@@ -13345,7 +13316,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F70" t="s">
         <v>154</v>
       </c>
@@ -13368,7 +13339,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F71" t="s">
         <v>154</v>
       </c>
@@ -13391,7 +13362,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
         <v>154</v>
       </c>
@@ -13414,7 +13385,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="73" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
         <v>154</v>
       </c>
@@ -13437,7 +13408,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="74" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
         <v>154</v>
       </c>
@@ -13460,7 +13431,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="75" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
         <v>154</v>
       </c>
@@ -13483,7 +13454,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="76" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
         <v>154</v>
       </c>
@@ -13506,7 +13477,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="77" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F77" t="s">
         <v>154</v>
       </c>
@@ -13529,7 +13500,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="78" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F78" t="s">
         <v>154</v>
       </c>
@@ -13552,7 +13523,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="79" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F79" t="s">
         <v>154</v>
       </c>
@@ -13575,7 +13546,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F80" t="s">
         <v>154</v>
       </c>
@@ -13598,7 +13569,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="81" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
         <v>154</v>
       </c>
@@ -13621,7 +13592,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="82" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
         <v>154</v>
       </c>
@@ -13644,7 +13615,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="83" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F83" t="s">
         <v>154</v>
       </c>
@@ -13667,7 +13638,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="84" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F84" t="s">
         <v>154</v>
       </c>
@@ -13690,7 +13661,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="85" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
         <v>154</v>
       </c>
@@ -13713,7 +13684,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="86" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
         <v>154</v>
       </c>
@@ -13736,7 +13707,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="87" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F87" t="s">
         <v>154</v>
       </c>
@@ -13759,7 +13730,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="88" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F88" t="s">
         <v>154</v>
       </c>
@@ -13782,7 +13753,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="89" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F89" t="s">
         <v>154</v>
       </c>
@@ -13805,7 +13776,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F90" t="s">
         <v>154</v>
       </c>
@@ -13828,7 +13799,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="91" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F91" t="s">
         <v>154</v>
       </c>
@@ -13851,7 +13822,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="92" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F92" t="s">
         <v>154</v>
       </c>
@@ -13874,7 +13845,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="93" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F93" t="s">
         <v>154</v>
       </c>
@@ -13897,7 +13868,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="94" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F94" t="s">
         <v>154</v>
       </c>
@@ -13920,7 +13891,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="95" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F95" t="s">
         <v>154</v>
       </c>
@@ -13943,7 +13914,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F96" t="s">
         <v>154</v>
       </c>
@@ -13966,7 +13937,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="97" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F97" t="s">
         <v>154</v>
       </c>
@@ -13989,7 +13960,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="98" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F98" t="s">
         <v>154</v>
       </c>
@@ -14012,7 +13983,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="99" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F99" t="s">
         <v>154</v>
       </c>
@@ -14035,7 +14006,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="100" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F100" t="s">
         <v>154</v>
       </c>
@@ -14058,7 +14029,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="101" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F101" t="s">
         <v>154</v>
       </c>
@@ -14081,7 +14052,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="102" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F102" t="s">
         <v>154</v>
       </c>
@@ -14104,7 +14075,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="103" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F103" t="s">
         <v>154</v>
       </c>
@@ -14127,7 +14098,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="104" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F104" t="s">
         <v>154</v>
       </c>
@@ -14150,7 +14121,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="105" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F105" t="s">
         <v>154</v>
       </c>
@@ -14173,7 +14144,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="106" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F106" t="s">
         <v>154</v>
       </c>
@@ -14196,7 +14167,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="107" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F107" t="s">
         <v>154</v>
       </c>
@@ -14219,7 +14190,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="108" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F108" t="s">
         <v>154</v>
       </c>
@@ -14242,7 +14213,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="109" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F109" t="s">
         <v>154</v>
       </c>
@@ -14265,7 +14236,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="110" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F110" t="s">
         <v>154</v>
       </c>
@@ -14288,7 +14259,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="111" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F111" t="s">
         <v>154</v>
       </c>
@@ -14311,7 +14282,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="112" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F112" t="s">
         <v>154</v>
       </c>
@@ -14334,7 +14305,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="113" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F113" t="s">
         <v>154</v>
       </c>
@@ -14357,7 +14328,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="114" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F114" t="s">
         <v>154</v>
       </c>
@@ -14380,7 +14351,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="115" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F115" t="s">
         <v>154</v>
       </c>
@@ -14403,7 +14374,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="116" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F116" t="s">
         <v>154</v>
       </c>
@@ -14426,7 +14397,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="117" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F117" t="s">
         <v>154</v>
       </c>
@@ -14449,7 +14420,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="118" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F118" t="s">
         <v>154</v>
       </c>
@@ -14472,7 +14443,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="119" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F119" t="s">
         <v>154</v>
       </c>
@@ -14495,7 +14466,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="120" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F120" t="s">
         <v>154</v>
       </c>
@@ -14518,7 +14489,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="121" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F121" t="s">
         <v>154</v>
       </c>
@@ -14541,7 +14512,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="122" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F122" t="s">
         <v>154</v>
       </c>
@@ -14564,7 +14535,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="123" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F123" t="s">
         <v>154</v>
       </c>
@@ -14587,7 +14558,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="124" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="124" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F124" t="s">
         <v>154</v>
       </c>
@@ -14610,7 +14581,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="125" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="125" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F125" t="s">
         <v>154</v>
       </c>
@@ -14633,7 +14604,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="126" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F126" t="s">
         <v>154</v>
       </c>
@@ -14656,7 +14627,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="127" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="127" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F127" t="s">
         <v>154</v>
       </c>
@@ -14679,7 +14650,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="128" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="128" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F128" t="s">
         <v>154</v>
       </c>
@@ -14702,7 +14673,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="129" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="129" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F129" t="s">
         <v>154</v>
       </c>
@@ -14725,7 +14696,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="130" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="130" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F130" t="s">
         <v>154</v>
       </c>
@@ -14748,7 +14719,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="131" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="131" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F131" t="s">
         <v>154</v>
       </c>
@@ -14771,7 +14742,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="132" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="132" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F132" t="s">
         <v>154</v>
       </c>
@@ -14794,7 +14765,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="133" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="133" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F133" t="s">
         <v>154</v>
       </c>
@@ -14817,7 +14788,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="134" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="134" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F134" t="s">
         <v>154</v>
       </c>
@@ -14840,7 +14811,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="135" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="135" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F135" t="s">
         <v>154</v>
       </c>
@@ -14863,7 +14834,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="136" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="136" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F136" t="s">
         <v>154</v>
       </c>
@@ -14886,7 +14857,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="137" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="137" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F137" t="s">
         <v>154</v>
       </c>
@@ -14909,7 +14880,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="138" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="138" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F138" t="s">
         <v>154</v>
       </c>
@@ -14932,7 +14903,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="139" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="139" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F139" t="s">
         <v>154</v>
       </c>
@@ -14955,7 +14926,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="140" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="140" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F140" t="s">
         <v>154</v>
       </c>
@@ -14978,7 +14949,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="141" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="141" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F141" t="s">
         <v>154</v>
       </c>
@@ -15001,7 +14972,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="142" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="142" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F142" t="s">
         <v>154</v>
       </c>
@@ -15024,7 +14995,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="143" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="143" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F143" t="s">
         <v>154</v>
       </c>
@@ -15047,7 +15018,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="144" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="144" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F144" t="s">
         <v>154</v>
       </c>
@@ -15070,7 +15041,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="145" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="145" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F145" t="s">
         <v>154</v>
       </c>
@@ -15093,7 +15064,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="146" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="146" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F146" t="s">
         <v>154</v>
       </c>
@@ -15116,7 +15087,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="147" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="147" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F147" t="s">
         <v>154</v>
       </c>
@@ -15139,7 +15110,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="148" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="148" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F148" t="s">
         <v>154</v>
       </c>
@@ -15162,7 +15133,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="149" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="149" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F149" t="s">
         <v>154</v>
       </c>
@@ -15185,7 +15156,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="150" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="150" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F150" t="s">
         <v>154</v>
       </c>
@@ -15208,7 +15179,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="151" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="151" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F151" t="s">
         <v>154</v>
       </c>
@@ -15231,7 +15202,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="152" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="152" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F152" t="s">
         <v>154</v>
       </c>
@@ -15254,7 +15225,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="153" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="153" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F153" t="s">
         <v>154</v>
       </c>
@@ -15277,7 +15248,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="154" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="154" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F154" t="s">
         <v>154</v>
       </c>
@@ -15300,7 +15271,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="155" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="155" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F155" t="s">
         <v>154</v>
       </c>
@@ -15323,7 +15294,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="156" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="156" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F156" t="s">
         <v>154</v>
       </c>
@@ -15346,7 +15317,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="157" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="157" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F157" t="s">
         <v>154</v>
       </c>
@@ -15369,7 +15340,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="158" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="158" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F158" t="s">
         <v>154</v>
       </c>
@@ -15392,7 +15363,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="159" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F159" t="s">
         <v>154</v>
       </c>
@@ -15415,7 +15386,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="160" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F160" t="s">
         <v>154</v>
       </c>
@@ -15438,7 +15409,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="161" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="161" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F161" t="s">
         <v>154</v>
       </c>
@@ -15461,7 +15432,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="162" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="162" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F162" t="s">
         <v>154</v>
       </c>
@@ -15484,7 +15455,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="163" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="163" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F163" t="s">
         <v>154</v>
       </c>
@@ -15507,7 +15478,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="164" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="164" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F164" t="s">
         <v>154</v>
       </c>
@@ -15530,7 +15501,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="165" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="165" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F165" t="s">
         <v>154</v>
       </c>
@@ -15553,7 +15524,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="166" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="166" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F166" t="s">
         <v>154</v>
       </c>
@@ -15576,7 +15547,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="167" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="167" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F167" t="s">
         <v>154</v>
       </c>
@@ -15599,7 +15570,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="168" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="168" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F168" t="s">
         <v>154</v>
       </c>
@@ -15622,7 +15593,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="169" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="169" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F169" t="s">
         <v>154</v>
       </c>
@@ -15645,7 +15616,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="170" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="170" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F170" t="s">
         <v>154</v>
       </c>
@@ -15668,7 +15639,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="171" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="171" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F171" t="s">
         <v>154</v>
       </c>
@@ -15691,7 +15662,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="172" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="172" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F172" t="s">
         <v>154</v>
       </c>
@@ -15714,7 +15685,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="173" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="173" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F173" t="s">
         <v>154</v>
       </c>
@@ -15737,7 +15708,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="174" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="174" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F174" t="s">
         <v>154</v>
       </c>
@@ -15760,7 +15731,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="175" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="175" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F175" t="s">
         <v>154</v>
       </c>
@@ -15783,7 +15754,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="176" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="176" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F176" t="s">
         <v>154</v>
       </c>
@@ -15806,7 +15777,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="177" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="177" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F177" t="s">
         <v>154</v>
       </c>
@@ -15829,7 +15800,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="178" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="178" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F178" t="s">
         <v>154</v>
       </c>
@@ -15852,7 +15823,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="179" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="179" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F179" t="s">
         <v>154</v>
       </c>
@@ -15875,7 +15846,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="180" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="180" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F180" t="s">
         <v>154</v>
       </c>
@@ -15898,7 +15869,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="181" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="181" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F181" t="s">
         <v>154</v>
       </c>
@@ -15921,7 +15892,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="182" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="182" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F182" t="s">
         <v>154</v>
       </c>
@@ -15944,7 +15915,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="183" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="183" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F183" t="s">
         <v>154</v>
       </c>
@@ -15967,7 +15938,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="184" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="184" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F184" t="s">
         <v>154</v>
       </c>
@@ -15990,7 +15961,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="185" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="185" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F185" t="s">
         <v>154</v>
       </c>
@@ -16013,7 +15984,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="186" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="186" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F186" t="s">
         <v>154</v>
       </c>
@@ -16036,7 +16007,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="187" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="187" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F187" t="s">
         <v>154</v>
       </c>
@@ -16059,7 +16030,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="188" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="188" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F188" t="s">
         <v>154</v>
       </c>
@@ -16082,7 +16053,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="189" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="189" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F189" t="s">
         <v>154</v>
       </c>
@@ -16105,7 +16076,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="190" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="190" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F190" t="s">
         <v>154</v>
       </c>
@@ -16128,7 +16099,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="191" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="191" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F191" t="s">
         <v>154</v>
       </c>
@@ -16151,7 +16122,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="192" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="192" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F192" t="s">
         <v>154</v>
       </c>
@@ -16174,7 +16145,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="193" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="193" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F193" t="s">
         <v>154</v>
       </c>
@@ -16197,7 +16168,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="194" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="194" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F194" t="s">
         <v>154</v>
       </c>
@@ -16220,7 +16191,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="195" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="195" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F195" t="s">
         <v>154</v>
       </c>
@@ -16243,7 +16214,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="196" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="196" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F196" t="s">
         <v>154</v>
       </c>
@@ -16266,7 +16237,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="197" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="197" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F197" t="s">
         <v>154</v>
       </c>
@@ -16289,7 +16260,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="198" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="198" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F198" t="s">
         <v>154</v>
       </c>
@@ -16312,7 +16283,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="199" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="199" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F199" t="s">
         <v>154</v>
       </c>
@@ -16335,7 +16306,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="200" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="200" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F200" t="s">
         <v>154</v>
       </c>
@@ -16358,7 +16329,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="201" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="201" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F201" t="s">
         <v>154</v>
       </c>
@@ -16381,7 +16352,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="202" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="202" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F202" t="s">
         <v>154</v>
       </c>
@@ -16404,7 +16375,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="203" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="203" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F203" t="s">
         <v>154</v>
       </c>
@@ -16427,7 +16398,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="204" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="204" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F204" t="s">
         <v>154</v>
       </c>
@@ -16450,7 +16421,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="205" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="205" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F205" t="s">
         <v>154</v>
       </c>
@@ -16473,7 +16444,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="206" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="206" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F206" t="s">
         <v>154</v>
       </c>
@@ -16496,7 +16467,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="207" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="207" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F207" t="s">
         <v>154</v>
       </c>
@@ -16519,7 +16490,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="208" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="208" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F208" t="s">
         <v>154</v>
       </c>
@@ -16542,7 +16513,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="209" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="209" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F209" t="s">
         <v>154</v>
       </c>
@@ -16565,7 +16536,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="210" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="210" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F210" t="s">
         <v>154</v>
       </c>
@@ -16588,7 +16559,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="211" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="211" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F211" t="s">
         <v>154</v>
       </c>
@@ -16611,7 +16582,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="212" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="212" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F212" t="s">
         <v>154</v>
       </c>
@@ -16634,7 +16605,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="213" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="213" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F213" t="s">
         <v>154</v>
       </c>
@@ -16657,7 +16628,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="214" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="214" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F214" t="s">
         <v>154</v>
       </c>
@@ -16680,7 +16651,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="215" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="215" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F215" t="s">
         <v>154</v>
       </c>
@@ -16703,7 +16674,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="216" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="216" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F216" t="s">
         <v>154</v>
       </c>
@@ -16739,18 +16710,18 @@
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.7265625" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" customWidth="1"/>
-    <col min="12" max="12" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="25" t="s">
         <v>150</v>
       </c>
@@ -16758,7 +16729,7 @@
       <c r="J3" s="26"/>
       <c r="K3" s="26"/>
     </row>
-    <row r="4" spans="3:14" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:14" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="27" t="s">
         <v>65</v>
       </c>
@@ -16791,7 +16762,7 @@
       </c>
       <c r="N4" s="29"/>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5" s="28" t="s">
         <v>153</v>
       </c>
@@ -16807,7 +16778,7 @@
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>154</v>
       </c>
@@ -16824,7 +16795,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>154</v>
       </c>
@@ -16841,7 +16812,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>154</v>
       </c>
@@ -16858,7 +16829,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>154</v>
       </c>
@@ -16875,7 +16846,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>154</v>
       </c>
@@ -16892,7 +16863,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>154</v>
       </c>
@@ -16909,7 +16880,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>154</v>
       </c>
@@ -16926,7 +16897,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>154</v>
       </c>
@@ -16943,7 +16914,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>154</v>
       </c>
@@ -16960,7 +16931,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>154</v>
       </c>
@@ -16977,7 +16948,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>154</v>
       </c>
@@ -16994,7 +16965,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>154</v>
       </c>
@@ -17011,7 +16982,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>154</v>
       </c>
@@ -17028,7 +16999,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>154</v>
       </c>
@@ -17045,7 +17016,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>154</v>
       </c>
@@ -17062,7 +17033,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>154</v>
       </c>
@@ -17079,7 +17050,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>154</v>
       </c>
@@ -17096,7 +17067,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>154</v>
       </c>
@@ -17113,7 +17084,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>154</v>
       </c>
@@ -17130,7 +17101,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>154</v>
       </c>
@@ -17147,7 +17118,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>154</v>
       </c>
@@ -17164,7 +17135,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>154</v>
       </c>
@@ -17181,7 +17152,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>154</v>
       </c>
@@ -17198,7 +17169,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>154</v>
       </c>
@@ -17215,7 +17186,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>154</v>
       </c>
@@ -17232,7 +17203,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>154</v>
       </c>
@@ -17249,7 +17220,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>154</v>
       </c>
@@ -17266,7 +17237,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>154</v>
       </c>

</xml_diff>

<commit_message>
Make hLED demands consistent with other demands
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED-Halfway.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED-Halfway.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-IE\2022-gas-study\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A4AB39-BE9E-489C-ACC6-7E2D8E51B002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BE28FC-0844-4206-897C-C1523EB8D675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="3390" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BY-Demands" sheetId="5" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Residential" sheetId="8" r:id="rId5"/>
     <sheet name="Services" sheetId="9" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="1" hidden="1">#REF!</definedName>
@@ -81,6 +84,73 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>vahid Aryanpur</author>
+    <author>tc={8DE729B7-ABD0-4D53-BC2E-AA72D346828F}</author>
+    <author>tc={B22842B4-E905-45E3-A282-CCE6064177FC}</author>
+    <author>tc={65328121-E0AA-4F0D-920A-29BDC2555B3E}</author>
+  </authors>
+  <commentList>
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{0657B891-7379-4F39-874C-BE95A2807F6B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>vahid Aryanpur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Updated, based on proportion of total fuel consumption</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="1" shapeId="0" xr:uid="{8DE729B7-ABD0-4D53-BC2E-AA72D346828F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</t>
+      </text>
+    </comment>
+    <comment ref="I20" authorId="2" shapeId="0" xr:uid="{B22842B4-E905-45E3-A282-CCE6064177FC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</t>
+      </text>
+    </comment>
+    <comment ref="J20" authorId="3" shapeId="0" xr:uid="{65328121-E0AA-4F0D-920A-29BDC2555B3E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -674,7 +744,7 @@
     <numFmt numFmtId="165" formatCode="\Te\x\t"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -774,6 +844,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1076,6 +1165,45 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover"/>
+      <sheetName val="BY-Demands"/>
+      <sheetName val="REG_TRA_DEMANDS"/>
+      <sheetName val="Regions"/>
+      <sheetName val="DEMANDS"/>
+      <sheetName val="Residential"/>
+      <sheetName val="Services"/>
+      <sheetName val="TRA-2021"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7">
+        <row r="11">
+          <cell r="C11">
+            <v>0.93264803405429875</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Balyk, Olexandr" id="{FEAD16CF-A605-4623-BB61-3A2A181D70B2}" userId="Balyk, Olexandr" providerId="None"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1337,6 +1465,26 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H20" dT="2022-10-12T22:37:02.29" personId="{FEAD16CF-A605-4623-BB61-3A2A181D70B2}" id="{8DE729B7-ABD0-4D53-BC2E-AA72D346828F}">
+    <text>Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</text>
+  </threadedComment>
+  <threadedComment ref="I20" dT="2022-10-12T22:37:46.05" personId="{FEAD16CF-A605-4623-BB61-3A2A181D70B2}" id="{B22842B4-E905-45E3-A282-CCE6064177FC}">
+    <text>Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</text>
+  </threadedComment>
+  <threadedComment ref="J20" dT="2022-10-12T22:37:54.36" personId="{FEAD16CF-A605-4623-BB61-3A2A181D70B2}" id="{65328121-E0AA-4F0D-920A-29BDC2555B3E}">
+    <text>Sum of Eurostat tables: 
+1) ROAD_GO_TA_TOTT
+2) RAIL_GO_TOTAL</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0226CF39-0357-4B21-823B-1B3093B14EE8}">
   <dimension ref="C4:AK42"/>
@@ -4149,107 +4297,107 @@
       </c>
       <c r="G6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.20300060063434958</v>
+        <v>0.17791021665128046</v>
       </c>
       <c r="H6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>4.0584633282751126</v>
+        <v>3.5568470622668977</v>
       </c>
       <c r="I6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.74848244469808678</v>
+        <v>0.65597182215127059</v>
       </c>
       <c r="J6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.34724754504054051</v>
+        <v>0.30432858709155108</v>
       </c>
       <c r="K6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.27376982026764263</v>
+        <v>0.23993253164866168</v>
       </c>
       <c r="L6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.13755999795611623</v>
+        <v>0.12055791442215673</v>
       </c>
       <c r="M6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.39445499612536866</v>
+        <v>0.34570131123035525</v>
       </c>
       <c r="N6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.64928302501009705</v>
+        <v>0.56903321116577554</v>
       </c>
       <c r="O6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.26877256463954802</v>
+        <v>0.2355529247476085</v>
       </c>
       <c r="P6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.30465079595834027</v>
+        <v>0.26699669332289716</v>
       </c>
       <c r="Q6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.53022575007917072</v>
+        <v>0.46469112788778127</v>
       </c>
       <c r="R6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46901260006304341</v>
+        <v>0.41104377538121051</v>
       </c>
       <c r="S6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.41278839282092511</v>
+        <v>0.36176874437029644</v>
       </c>
       <c r="T6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.7456271862846215</v>
+        <v>1.5298718818259087</v>
       </c>
       <c r="U6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.53447019407874841</v>
+        <v>0.46841096885952921</v>
       </c>
       <c r="V6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.6373124074899349</v>
+        <v>0.5585421330615401</v>
       </c>
       <c r="W6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.58101868325410067</v>
+        <v>0.50920617718944683</v>
       </c>
       <c r="X6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.38581506771754165</v>
+        <v>0.33812925710793035</v>
       </c>
       <c r="Y6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.86232255454765427</v>
+        <v>0.75574156935227998</v>
       </c>
       <c r="Z6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.11067259735658087</v>
+        <v>9.699373160247457E-2</v>
       </c>
       <c r="AA6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46181565455091583</v>
+        <v>0.40473635495344346</v>
       </c>
       <c r="AB6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.24158039942260146</v>
+        <v>0.21172164548120723</v>
       </c>
       <c r="AC6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.21298903965802496</v>
+        <v>0.18666410873414702</v>
       </c>
       <c r="AD6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.2375678491388247</v>
+        <v>0.2082050367220207</v>
       </c>
       <c r="AE6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46084064726442553</v>
+        <v>0.40388185621287809</v>
       </c>
       <c r="AF6" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E6,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F6,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E6,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.22102568255169014</v>
+        <v>0.19370744197499956</v>
       </c>
     </row>
     <row r="7" spans="2:32" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -4845,107 +4993,107 @@
       </c>
       <c r="G12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46342451965761583</v>
+        <v>0.40588049118145847</v>
       </c>
       <c r="H12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>8.1155755961155194</v>
+        <v>7.107853964234006</v>
       </c>
       <c r="I12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.6525894242319275</v>
+        <v>1.4473852348686691</v>
       </c>
       <c r="J12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.7848468237617493</v>
+        <v>0.68739136756505304</v>
       </c>
       <c r="K12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.59049140670441203</v>
+        <v>0.51716931673940703</v>
       </c>
       <c r="L12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.3042181315799129</v>
+        <v>0.26644296845403537</v>
       </c>
       <c r="M12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.81942741912586947</v>
+        <v>0.71767804519295675</v>
       </c>
       <c r="N12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.4226196661202095</v>
+        <v>1.2459711222787131</v>
       </c>
       <c r="O12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.60289301217975388</v>
+        <v>0.52803099864930969</v>
       </c>
       <c r="P12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.68057420745305641</v>
+        <v>0.59606641834696639</v>
       </c>
       <c r="Q12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.2070161615941664</v>
+        <v>1.057139386784598</v>
       </c>
       <c r="R12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.0242599623466919</v>
+        <v>0.89707626372882077</v>
       </c>
       <c r="S12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.9289528309484778</v>
+        <v>0.81360354343861541</v>
       </c>
       <c r="T12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>3.7541899081155736</v>
+        <v>3.2880272390856486</v>
       </c>
       <c r="U12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.2287453474819043</v>
+        <v>1.0761704312524312</v>
       </c>
       <c r="V12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.3838834420094299</v>
+        <v>1.2120448257585934</v>
       </c>
       <c r="W12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.3422029707145537</v>
+        <v>1.1755398730764657</v>
       </c>
       <c r="X12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.84676500468112548</v>
+        <v>0.74162108700930296</v>
       </c>
       <c r="Y12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.8958558850984162</v>
+        <v>1.6604449812485407</v>
       </c>
       <c r="Z12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.248475056333125</v>
+        <v>0.21762158373782103</v>
       </c>
       <c r="AA12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.0499837149519835</v>
+        <v>0.9196058643424867</v>
       </c>
       <c r="AB12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.56534360393881622</v>
+        <v>0.49514414952085861</v>
       </c>
       <c r="AC12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46120460967074761</v>
+        <v>0.40393623031991749</v>
       </c>
       <c r="AD12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.50113203851603993</v>
+        <v>0.4389058181253126</v>
       </c>
       <c r="AE12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.92291572480430029</v>
+        <v>0.80831607265713046</v>
       </c>
       <c r="AF12" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E12,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F12,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E12,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.50756865536512175</v>
+        <v>0.44454319184516294</v>
       </c>
     </row>
     <row r="13" spans="2:32" x14ac:dyDescent="0.2">
@@ -5541,107 +5689,107 @@
       </c>
       <c r="G18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.3949319127195085</v>
+        <v>0.34871475560546433</v>
       </c>
       <c r="H18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>7.0354598059455613</v>
+        <v>6.2121306680648631</v>
       </c>
       <c r="I18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.4215064973824205</v>
+        <v>1.2551537995825381</v>
       </c>
       <c r="J18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.68451237102108609</v>
+        <v>0.6044068774433683</v>
       </c>
       <c r="K18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.5085872808789732</v>
+        <v>0.44906953235181829</v>
       </c>
       <c r="L18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.2618778295465003</v>
+        <v>0.23123141075118878</v>
       </c>
       <c r="M18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.71158722914103401</v>
+        <v>0.62831328315096635</v>
       </c>
       <c r="N18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.2100639919064762</v>
+        <v>1.0684554871723726</v>
       </c>
       <c r="O18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.5215587975249425</v>
+        <v>0.46052304905013597</v>
       </c>
       <c r="P18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.57800689839391617</v>
+        <v>0.51036527517810415</v>
       </c>
       <c r="Q18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.0273437110504584</v>
+        <v>0.90711816286219038</v>
       </c>
       <c r="R18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.87971877108373875</v>
+        <v>0.77676912495517314</v>
       </c>
       <c r="S18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.78875759816931479</v>
+        <v>0.69645274088780662</v>
       </c>
       <c r="T18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>3.2162421821708547</v>
+        <v>2.8398594046266692</v>
       </c>
       <c r="U18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.0696076988780558</v>
+        <v>0.94443618075729097</v>
       </c>
       <c r="V18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.1848865981492651</v>
+        <v>1.0462244938591938</v>
       </c>
       <c r="W18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.1462954859601473</v>
+        <v>1.0121495310057134</v>
       </c>
       <c r="X18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.72187705815118308</v>
+        <v>0.63739893840679929</v>
       </c>
       <c r="Y18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.6400933547220824</v>
+        <v>1.4481603915565415</v>
       </c>
       <c r="Z18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.21158507026178613</v>
+        <v>0.18682419346168758</v>
       </c>
       <c r="AA18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.90946181001663118</v>
+        <v>0.80303146592687813</v>
       </c>
       <c r="AB18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.47670587805089104</v>
+        <v>0.42091907087353819</v>
       </c>
       <c r="AC18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.39733782511006455</v>
+        <v>0.35083911457535288</v>
       </c>
       <c r="AD18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.42495116243643605</v>
+        <v>0.37522098361933615</v>
       </c>
       <c r="AE18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.78279105429979845</v>
+        <v>0.69118443559198872</v>
       </c>
       <c r="AF18" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E18,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F18,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E18,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.45217630306421169</v>
+        <v>0.39926008492914083</v>
       </c>
     </row>
     <row r="19" spans="4:32" x14ac:dyDescent="0.2">
@@ -6005,107 +6153,107 @@
       </c>
       <c r="G22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.2178146269505315</v>
+        <v>0.19157023231298867</v>
       </c>
       <c r="H22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>3.2532352952549441</v>
+        <v>2.8612543152225762</v>
       </c>
       <c r="I22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.59035591066396753</v>
+        <v>0.51922417028002199</v>
       </c>
       <c r="J22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.37964907365901629</v>
+        <v>0.3339053132312666</v>
       </c>
       <c r="K22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.2704057614094616</v>
+        <v>0.23782468265432868</v>
       </c>
       <c r="L22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.13049216248614431</v>
+        <v>0.11476921560539823</v>
       </c>
       <c r="M22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.34195983528392676</v>
+        <v>0.30075723565585522</v>
       </c>
       <c r="N22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.5291116374087359</v>
+        <v>0.4653591942698963</v>
       </c>
       <c r="O22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.24890023926754198</v>
+        <v>0.21891035201263434</v>
       </c>
       <c r="P22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.28340932312027484</v>
+        <v>0.24926145057351232</v>
       </c>
       <c r="Q22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.57281742387914369</v>
+        <v>0.50379888854010457</v>
       </c>
       <c r="R22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.3778873214697962</v>
+        <v>0.33235583383728884</v>
       </c>
       <c r="S22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.37186096343983388</v>
+        <v>0.32705558920283034</v>
       </c>
       <c r="T22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.9896591411313085</v>
+        <v>1.7499259311761122</v>
       </c>
       <c r="U22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.54135919368811836</v>
+        <v>0.47613104754052427</v>
       </c>
       <c r="V22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.60997441370730043</v>
+        <v>0.53647884797665768</v>
       </c>
       <c r="W22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.49935221643128408</v>
+        <v>0.43918547366184335</v>
       </c>
       <c r="X22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.46383071132724779</v>
+        <v>0.40794394006900198</v>
       </c>
       <c r="Y22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.74064511268734978</v>
+        <v>0.6514050882873873</v>
       </c>
       <c r="Z22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>9.8775540783756666E-2</v>
+        <v>8.6874116581173791E-2</v>
       </c>
       <c r="AA22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.41714780682374364</v>
+        <v>0.36688583949060316</v>
       </c>
       <c r="AB22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.18524594530412608</v>
+        <v>0.1629257376962582</v>
       </c>
       <c r="AC22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.20201145503880613</v>
+        <v>0.17767117807225169</v>
       </c>
       <c r="AD22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.23481230791235341</v>
+        <v>0.20651986970064592</v>
       </c>
       <c r="AE22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.49070889678091939</v>
+        <v>0.43158358403414709</v>
       </c>
       <c r="AF22" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E22,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F22,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E22,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.18922217409036649</v>
+        <v>0.16642287231469072</v>
       </c>
     </row>
     <row r="23" spans="4:32" x14ac:dyDescent="0.2">
@@ -6121,107 +6269,107 @@
       </c>
       <c r="G23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.17991488188042462</v>
+        <v>0.17598869695867239</v>
       </c>
       <c r="H23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>2.6871723541686299</v>
+        <v>2.6285316488038659</v>
       </c>
       <c r="I23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.48763398226070803</v>
+        <v>0.47699261024925638</v>
       </c>
       <c r="J23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.3135901348759621</v>
+        <v>0.30674682738359726</v>
       </c>
       <c r="K23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.22335515894815736</v>
+        <v>0.21848100041223001</v>
       </c>
       <c r="L23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.10778652622510916</v>
+        <v>0.10543435930256223</v>
       </c>
       <c r="M23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.2824588239748011</v>
+        <v>0.27629487820158383</v>
       </c>
       <c r="N23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.43704621254646414</v>
+        <v>0.42750879000601366</v>
       </c>
       <c r="O23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.20559159765702764</v>
+        <v>0.20110508368818067</v>
       </c>
       <c r="P23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.23409610092244049</v>
+        <v>0.22898754863328891</v>
       </c>
       <c r="Q23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.47314719217489071</v>
+        <v>0.4628219575290925</v>
       </c>
       <c r="R23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.31213492756751032</v>
+        <v>0.30532337627525935</v>
       </c>
       <c r="S23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.30715715583422787</v>
+        <v>0.30045423175568414</v>
       </c>
       <c r="T23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.643458450750628</v>
+        <v>1.6075941480235647</v>
       </c>
       <c r="U23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.44716269403431846</v>
+        <v>0.4374045050032716</v>
       </c>
       <c r="V23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.50383886577623815</v>
+        <v>0.4928438633777254</v>
       </c>
       <c r="W23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.41246493081645397</v>
+        <v>0.40346393225981741</v>
       </c>
       <c r="X23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.38312416759737483</v>
+        <v>0.37476345660861177</v>
       </c>
       <c r="Y23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.61177286314532875</v>
+        <v>0.59842247564144924</v>
       </c>
       <c r="Z23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>8.1588596696128737E-2</v>
+        <v>7.9808132985805066E-2</v>
       </c>
       <c r="AA23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.34456408847334713</v>
+        <v>0.33704485318495958</v>
       </c>
       <c r="AB23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.15301315083761008</v>
+        <v>0.14967402780693329</v>
       </c>
       <c r="AC23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.16686146187994025</v>
+        <v>0.16322013466560803</v>
       </c>
       <c r="AD23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.1939549663563945</v>
+        <v>0.18972239228331952</v>
       </c>
       <c r="AE23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.40532554878448751</v>
+        <v>0.39648034909113317</v>
       </c>
       <c r="AF23" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E23,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F23,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E23,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.15629751581539669</v>
+        <v>0.15288671986851338</v>
       </c>
     </row>
     <row r="24" spans="4:32" x14ac:dyDescent="0.2">
@@ -6237,107 +6385,107 @@
       </c>
       <c r="G24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!G$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.19572571146618054</v>
+        <v>0.19228961557590898</v>
       </c>
       <c r="H24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!H$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>2.9233197129377184</v>
+        <v>2.871998878406937</v>
       </c>
       <c r="I24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!I$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.53048701205549609</v>
+        <v>0.52117395743271944</v>
       </c>
       <c r="J24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!J$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.34114827865193581</v>
+        <v>0.33515919224388002</v>
       </c>
       <c r="K24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!K$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.24298349829573737</v>
+        <v>0.23871776032169476</v>
       </c>
       <c r="L24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!L$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.11725875209088529</v>
+        <v>0.11520019620091229</v>
       </c>
       <c r="M24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!M$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.30728116376227216</v>
+        <v>0.30188663722790898</v>
       </c>
       <c r="N24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!N$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.47545361451038171</v>
+        <v>0.46710670802274745</v>
       </c>
       <c r="O24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!O$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.22365888414741908</v>
+        <v>0.21973240271130756</v>
       </c>
       <c r="P24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!P$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.25466834886374512</v>
+        <v>0.25019747551574262</v>
       </c>
       <c r="Q24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Q$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.51472713012259241</v>
+        <v>0.50569075077735171</v>
       </c>
       <c r="R24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!R$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.33956518845505695</v>
+        <v>0.33360389425518211</v>
       </c>
       <c r="S24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!S$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.3341499726383883</v>
+        <v>0.32828374617730566</v>
       </c>
       <c r="T24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!T$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>1.7878847551480515</v>
+        <v>1.7564972414002475</v>
       </c>
       <c r="U24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!U$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.48645912731760305</v>
+        <v>0.47791901168517154</v>
       </c>
       <c r="V24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!V$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.54811597260702893</v>
+        <v>0.53849342978034132</v>
       </c>
       <c r="W24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!W$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.44871214207035037</v>
+        <v>0.44083470003305669</v>
       </c>
       <c r="X24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!X$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.41679292729504486</v>
+        <v>0.40947584844094537</v>
       </c>
       <c r="Y24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Y$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.66553515553206655</v>
+        <v>0.65385124034471442</v>
       </c>
       <c r="Z24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!Z$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>8.8758561654118218E-2</v>
+        <v>8.7200345686264502E-2</v>
       </c>
       <c r="AA24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AA$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.37484420775688798</v>
+        <v>0.36826356675618782</v>
       </c>
       <c r="AB24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AB$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.16645986979152586</v>
+        <v>0.1635375553434078</v>
       </c>
       <c r="AC24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AC$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.18152516346282133</v>
+        <v>0.17833836769908104</v>
       </c>
       <c r="AD24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AD$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.21099963152428264</v>
+        <v>0.2072953917425068</v>
       </c>
       <c r="AE24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AE$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.44094535472607599</v>
+        <v>0.43320426383996402</v>
       </c>
       <c r="AF24" s="14">
         <f>HLOOKUP(REG_TRA_DEMANDS!AF$3,'BY-Demands'!$J$5:$AK$14,MATCH($E24,'BY-Demands'!$I$5:$I$14,0),FALSE)*HLOOKUP(REG_TRA_DEMANDS!$F24,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)/HLOOKUP(2018,DEMANDS!$G$2:$CW$25,MATCH($E24,DEMANDS!$E$2:$E$25,0),FALSE)</f>
-        <v>0.17003286311633117</v>
+        <v>0.16704782237851226</v>
       </c>
     </row>
     <row r="25" spans="4:32" x14ac:dyDescent="0.2">
@@ -10938,11 +11086,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AN56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11720,8 +11868,9 @@
       <c r="I17" s="30">
         <v>10.76129175</v>
       </c>
-      <c r="J17" s="30">
-        <v>15.490769824884</v>
+      <c r="J17" s="1">
+        <f>G17*'[1]TRA-2021'!$C$11</f>
+        <v>13.576148085415543</v>
       </c>
       <c r="K17" s="30">
         <v>15.7055907873725</v>
@@ -11769,8 +11918,9 @@
       <c r="I18" s="30">
         <v>23.13677727</v>
       </c>
-      <c r="J18" s="30">
-        <v>33.305155123500498</v>
+      <c r="J18" s="1">
+        <f>G18*'[1]TRA-2021'!$C$11</f>
+        <v>29.169610469442279</v>
       </c>
       <c r="K18" s="30">
         <v>33.767020192851</v>
@@ -11818,8 +11968,9 @@
       <c r="I19" s="30">
         <v>19.908389740000001</v>
       </c>
-      <c r="J19" s="30">
-        <v>28.657924176035301</v>
+      <c r="J19" s="1">
+        <f>G19*'[1]TRA-2021'!$C$11</f>
+        <v>25.304212456246088</v>
       </c>
       <c r="K19" s="30">
         <v>29.055342956639201</v>
@@ -11862,13 +12013,16 @@
         <v>11.625551</v>
       </c>
       <c r="H20" s="30">
-        <v>14.23064449</v>
+        <f>(12444+72)/1000</f>
+        <v>12.516</v>
       </c>
       <c r="I20" s="30">
-        <v>11.754512350000001</v>
+        <f>(11424+74)/1000</f>
+        <v>11.497999999999999</v>
       </c>
       <c r="J20" s="30">
-        <v>12.787492999999998</v>
+        <f>(12493+70)/1000</f>
+        <v>12.563000000000001</v>
       </c>
       <c r="K20" s="30">
         <v>13.183905282999998</v>
@@ -12264,7 +12418,8 @@
         <v>14.3748</v>
       </c>
       <c r="K28" s="31">
-        <v>17.1311</v>
+        <f>600*8760/10^6*3.6</f>
+        <v>18.921600000000002</v>
       </c>
       <c r="L28" s="30">
         <v>25</v>
@@ -13027,6 +13182,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Synchronise DC projections between hLED and LED
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_Demands_LED-Halfway.xlsx
+++ b/SuppXLS/Scen_SYS_Demands_LED-Halfway.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BE28FC-0844-4206-897C-C1523EB8D675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01015876-40F1-4745-9986-BDBBBADE8EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -744,7 +744,7 @@
     <numFmt numFmtId="165" formatCode="\Te\x\t"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -857,12 +857,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1179,13 +1173,13 @@
       <sheetName val="TRA-2021"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
       <sheetData sheetId="7">
         <row r="11">
           <cell r="C11">
@@ -11090,7 +11084,7 @@
   <dimension ref="B1:AN56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11146,15 +11140,18 @@
         <v>2030</v>
       </c>
       <c r="M2" s="13">
+        <v>2031</v>
+      </c>
+      <c r="N2" s="13">
         <v>2050</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>185</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>186</v>
       </c>
     </row>
@@ -11191,17 +11188,17 @@
       <c r="L3" s="30">
         <v>1.1584060685789734</v>
       </c>
-      <c r="M3" s="30">
-        <f>AVERAGE(Q3:R3)</f>
+      <c r="N3" s="30">
+        <f>AVERAGE(R3:S3)</f>
         <v>9.7989935307649739E-2</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="30">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="30">
         <v>0.126438626203419</v>
       </c>
-      <c r="R3" s="30">
+      <c r="S3" s="30">
         <v>6.9541244411880462E-2</v>
       </c>
       <c r="T3" s="30"/>
@@ -11240,17 +11237,17 @@
       <c r="L4" s="30">
         <v>22.05783877515594</v>
       </c>
-      <c r="M4" s="30">
-        <f t="shared" ref="M4:M29" si="0">AVERAGE(Q4:R4)</f>
+      <c r="N4" s="30">
+        <f t="shared" ref="N4:N29" si="0">AVERAGE(R4:S4)</f>
         <v>26.346234207155959</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="30">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="30">
         <v>33.995140912459298</v>
       </c>
-      <c r="R4" s="30">
+      <c r="S4" s="30">
         <v>18.697327501852616</v>
       </c>
       <c r="T4" s="30"/>
@@ -11289,17 +11286,17 @@
       <c r="L5" s="30">
         <v>1.9434753073389506</v>
       </c>
-      <c r="M5" s="30">
+      <c r="N5" s="30">
         <f t="shared" si="0"/>
         <v>3.8534877653787154</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="30">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="R5" s="30">
         <v>4.9722422779080198</v>
       </c>
-      <c r="R5" s="30">
+      <c r="S5" s="30">
         <v>2.7347332528494115</v>
       </c>
       <c r="T5" s="30"/>
@@ -11338,17 +11335,17 @@
       <c r="L6" s="30">
         <v>5.2807562869892761</v>
       </c>
-      <c r="M6" s="30">
+      <c r="N6" s="30">
         <f t="shared" si="0"/>
         <v>5.9308505795404391</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="30">
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="R6" s="30">
         <v>7.6527104252134697</v>
       </c>
-      <c r="R6" s="30">
+      <c r="S6" s="30">
         <v>4.2089907338674086</v>
       </c>
       <c r="T6" s="30"/>
@@ -11387,17 +11384,17 @@
       <c r="L7" s="30">
         <v>1.22325956804396</v>
       </c>
-      <c r="M7" s="30">
+      <c r="N7" s="30">
         <f t="shared" si="0"/>
         <v>1.7912647554770649</v>
       </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="30">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="R7" s="30">
         <v>2.3113093619058902</v>
       </c>
-      <c r="R7" s="30">
+      <c r="S7" s="30">
         <v>1.2712201490482398</v>
       </c>
       <c r="T7" s="30"/>
@@ -11436,17 +11433,17 @@
       <c r="L8" s="30">
         <v>9.4725222533350699</v>
       </c>
-      <c r="M8" s="30">
+      <c r="N8" s="30">
         <f t="shared" si="0"/>
         <v>10.157935062437405</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="30">
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="R8" s="30">
         <v>13.107012983790201</v>
       </c>
-      <c r="R8" s="30">
+      <c r="S8" s="30">
         <v>7.2088571410846098</v>
       </c>
       <c r="T8" s="30"/>
@@ -11485,17 +11482,17 @@
       <c r="L9" s="30">
         <v>0.85675812345956381</v>
       </c>
-      <c r="M9" s="30">
+      <c r="N9" s="30">
         <f t="shared" si="0"/>
         <v>0.68793979220818868</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="30">
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="R9" s="30">
         <v>0.88766424801056598</v>
       </c>
-      <c r="R9" s="30">
+      <c r="S9" s="30">
         <v>0.48821533640581133</v>
       </c>
       <c r="T9" s="30"/>
@@ -11534,17 +11531,17 @@
       <c r="L10" s="30">
         <v>15.463248848798345</v>
       </c>
-      <c r="M10" s="30">
+      <c r="N10" s="30">
         <f t="shared" si="0"/>
         <v>16.853923637480463</v>
       </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="30">
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="R10" s="30">
         <v>24.822798092583323</v>
       </c>
-      <c r="R10" s="30">
+      <c r="S10" s="30">
         <v>8.8850491823775997</v>
       </c>
       <c r="T10" s="30"/>
@@ -11583,17 +11580,17 @@
       <c r="L11" s="30">
         <v>16.048363755990756</v>
       </c>
-      <c r="M11" s="30">
+      <c r="N11" s="30">
         <f t="shared" si="0"/>
         <v>16.844014653390236</v>
       </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="30">
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="R11" s="30">
         <v>21.7342124559874</v>
       </c>
-      <c r="R11" s="30">
+      <c r="S11" s="30">
         <v>11.953816850793071</v>
       </c>
       <c r="T11" s="30"/>
@@ -11632,17 +11629,17 @@
       <c r="L12" s="30">
         <v>1.8148484316492632</v>
       </c>
-      <c r="M12" s="30">
+      <c r="N12" s="30">
         <f t="shared" si="0"/>
         <v>1.3071809478517049</v>
       </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="30">
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="R12" s="30">
         <v>1.6866850940022</v>
       </c>
-      <c r="R12" s="30">
+      <c r="S12" s="30">
         <v>0.92767680170120992</v>
       </c>
       <c r="T12" s="30"/>
@@ -11681,17 +11678,17 @@
       <c r="L13" s="30">
         <v>7.1919298250215675</v>
       </c>
-      <c r="M13" s="30">
+      <c r="N13" s="30">
         <f t="shared" si="0"/>
         <v>12.686569622394671</v>
       </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="30">
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="R13" s="30">
         <v>16.369767254702801</v>
       </c>
-      <c r="R13" s="30">
+      <c r="S13" s="30">
         <v>9.0033719900865421</v>
       </c>
       <c r="T13" s="30"/>
@@ -11730,17 +11727,17 @@
       <c r="L14" s="30">
         <v>0.1326581724749025</v>
       </c>
-      <c r="M14" s="30">
+      <c r="N14" s="30">
         <f t="shared" si="0"/>
         <v>3.2628733640509965E-2</v>
       </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="30">
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="R14" s="30">
         <v>4.2101591794206403E-2</v>
       </c>
-      <c r="R14" s="30">
+      <c r="S14" s="30">
         <v>2.3155875486813523E-2</v>
       </c>
       <c r="T14" s="30"/>
@@ -11779,17 +11776,17 @@
       <c r="L15" s="30">
         <v>4.2494582874450408</v>
       </c>
-      <c r="M15" s="30">
+      <c r="N15" s="30">
         <f t="shared" si="0"/>
         <v>4.7394475614649956</v>
       </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="30">
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="R15" s="30">
         <v>6.1154162083419301</v>
       </c>
-      <c r="R15" s="30">
+      <c r="S15" s="30">
         <v>3.3634789145880619</v>
       </c>
       <c r="T15" s="30"/>
@@ -11828,17 +11825,17 @@
       <c r="L16" s="30">
         <v>3.5045513913327135</v>
       </c>
-      <c r="M16" s="30">
+      <c r="N16" s="30">
         <f t="shared" si="0"/>
         <v>4.5713249322390208</v>
       </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="30">
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="R16" s="30">
         <v>5.8984837835342203</v>
       </c>
-      <c r="R16" s="30">
+      <c r="S16" s="30">
         <v>3.2441660809438213</v>
       </c>
       <c r="T16" s="30"/>
@@ -11878,17 +11875,17 @@
       <c r="L17" s="30">
         <v>16.798154247711324</v>
       </c>
-      <c r="M17" s="30">
+      <c r="N17" s="30">
         <f t="shared" si="0"/>
         <v>19.808098215775729</v>
       </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="30">
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="R17" s="30">
         <v>21.065548257939199</v>
       </c>
-      <c r="R17" s="30">
+      <c r="S17" s="30">
         <v>18.550648173612263</v>
       </c>
       <c r="T17" s="30"/>
@@ -11928,17 +11925,17 @@
       <c r="L18" s="30">
         <v>30.018312954312446</v>
       </c>
-      <c r="M18" s="30">
+      <c r="N18" s="30">
         <f t="shared" si="0"/>
         <v>37.651251214826601</v>
       </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="30">
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="R18" s="30">
         <v>45.290928754569201</v>
       </c>
-      <c r="R18" s="30">
+      <c r="S18" s="30">
         <v>30.011573675084005</v>
       </c>
       <c r="T18" s="30"/>
@@ -11978,17 +11975,17 @@
       <c r="L19" s="30">
         <v>25.857221286837778</v>
       </c>
-      <c r="M19" s="30">
+      <c r="N19" s="30">
         <f t="shared" si="0"/>
         <v>32.379777214245621</v>
       </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="30">
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="R19" s="30">
         <v>38.971264277187501</v>
       </c>
-      <c r="R19" s="30">
+      <c r="S19" s="30">
         <v>25.788290151303741</v>
       </c>
       <c r="T19" s="30"/>
@@ -12030,17 +12027,17 @@
       <c r="L20" s="30">
         <v>11.939270188666665</v>
       </c>
-      <c r="M20" s="30">
+      <c r="N20" s="30">
         <f t="shared" si="0"/>
         <v>17.294083387740336</v>
       </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="30">
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="R20" s="30">
         <v>25.138166775480673</v>
       </c>
-      <c r="R20" s="30">
+      <c r="S20" s="30">
         <v>9.4499999999999993</v>
       </c>
       <c r="T20" s="30"/>
@@ -12080,17 +12077,17 @@
       <c r="L21" s="30">
         <v>0</v>
       </c>
-      <c r="M21" s="30">
+      <c r="N21" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="30">
+      <c r="O21">
         <v>0</v>
       </c>
       <c r="R21" s="30">
+        <v>0</v>
+      </c>
+      <c r="S21" s="30">
         <v>0</v>
       </c>
       <c r="T21" s="30"/>
@@ -12129,17 +12126,17 @@
       <c r="L22" s="30">
         <v>4.2785555697549427</v>
       </c>
-      <c r="M22" s="30">
+      <c r="N22" s="30">
         <f t="shared" si="0"/>
         <v>6.7763561055681549</v>
       </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="30">
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="R22" s="30">
         <v>10.039412402408599</v>
       </c>
-      <c r="R22" s="30">
+      <c r="S22" s="30">
         <v>3.5132998087277101</v>
       </c>
       <c r="T22" s="30"/>
@@ -12178,17 +12175,17 @@
       <c r="L23" s="30">
         <v>0</v>
       </c>
-      <c r="M23" s="30">
+      <c r="N23" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="30">
+      <c r="O23">
         <v>0</v>
       </c>
       <c r="R23" s="30">
+        <v>0</v>
+      </c>
+      <c r="S23" s="30">
         <v>0</v>
       </c>
       <c r="T23" s="30"/>
@@ -12227,17 +12224,17 @@
       <c r="L24" s="30">
         <v>0.23116440009552636</v>
       </c>
-      <c r="M24" s="30">
+      <c r="N24" s="30">
         <f t="shared" si="0"/>
         <v>0.23174660014328952</v>
       </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="30">
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="R24" s="30">
         <v>0.23</v>
       </c>
-      <c r="R24" s="30">
+      <c r="S24" s="30">
         <v>0.23349320028657899</v>
       </c>
       <c r="T24" s="30"/>
@@ -12276,17 +12273,17 @@
       <c r="L25" s="30">
         <v>47.451052484086929</v>
       </c>
-      <c r="M25" s="30">
+      <c r="N25" s="30">
         <f t="shared" si="0"/>
         <v>54.299091756130395</v>
       </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="30">
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="R25" s="30">
         <v>62.629819759999997</v>
       </c>
-      <c r="R25" s="30">
+      <c r="S25" s="30">
         <v>45.9683637522608</v>
       </c>
       <c r="T25" s="30"/>
@@ -12325,17 +12322,17 @@
       <c r="L26" s="30">
         <v>31.989398146398109</v>
       </c>
-      <c r="M26" s="30">
+      <c r="N26" s="30">
         <f t="shared" si="0"/>
         <v>40.081955186767516</v>
       </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="30">
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="R26" s="30">
         <v>47.391759323456121</v>
       </c>
-      <c r="R26" s="30">
+      <c r="S26" s="30">
         <v>32.772151050078904</v>
       </c>
       <c r="T26" s="30"/>
@@ -12374,17 +12371,17 @@
       <c r="L27" s="30">
         <v>64.414276297117567</v>
       </c>
-      <c r="M27" s="30">
+      <c r="N27" s="30">
         <f t="shared" si="0"/>
         <v>80.721923849501025</v>
       </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="30">
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="R27" s="30">
         <v>95.354503699002038</v>
       </c>
-      <c r="R27" s="30">
+      <c r="S27" s="30">
         <v>66.089343999999997</v>
       </c>
       <c r="T27" s="30"/>
@@ -12421,21 +12418,24 @@
         <f>600*8760/10^6*3.6</f>
         <v>18.921600000000002</v>
       </c>
-      <c r="L28" s="30">
-        <v>25</v>
-      </c>
-      <c r="M28" s="30">
+      <c r="L28" s="30"/>
+      <c r="M28" s="31">
+        <f>1491*8760/10^6*3.6</f>
+        <v>47.020175999999999</v>
+      </c>
+      <c r="N28" s="30">
         <f t="shared" si="0"/>
-        <v>35.15</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="30">
-        <v>40.299999999999997</v>
+        <v>47.020175999999999</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
       </c>
       <c r="R28" s="30">
-        <v>30</v>
+        <v>47.020175999999999</v>
+      </c>
+      <c r="S28" s="30">
+        <f>R28</f>
+        <v>47.020175999999999</v>
       </c>
       <c r="T28" s="30"/>
       <c r="U28" s="33"/>
@@ -12465,17 +12465,17 @@
       <c r="L29" s="30">
         <v>0.5</v>
       </c>
-      <c r="M29" s="30">
+      <c r="N29" s="30">
         <f t="shared" si="0"/>
         <v>0.5575</v>
       </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="30">
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="R29" s="30">
         <v>0.57499999999999996</v>
       </c>
-      <c r="R29" s="30">
+      <c r="S29" s="30">
         <v>0.54</v>
       </c>
       <c r="T29" s="30"/>

</xml_diff>